<commit_message>
Testcase login in progress
</commit_message>
<xml_diff>
--- a/src/com/qtpselenium/xls/Login Suite.xlsx
+++ b/src/com/qtpselenium/xls/Login Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>TCID</t>
   </si>
@@ -88,12 +88,22 @@
   </si>
   <si>
     <t>password$1</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,15 +469,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,7 +504,9 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -518,15 +530,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C3:C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -556,28 +568,36 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
   </sheetData>
@@ -595,9 +615,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Login test Case done
</commit_message>
<xml_diff>
--- a/src/com/qtpselenium/xls/Login Suite.xlsx
+++ b/src/com/qtpselenium/xls/Login Suite.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Checklogin" sheetId="2" r:id="rId2"/>
-    <sheet name="TestCase_A2" sheetId="3" r:id="rId3"/>
+    <sheet name="NewCustomerRegistration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>TCID</t>
   </si>
@@ -30,80 +30,97 @@
     <t>Y</t>
   </si>
   <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Login into application</t>
+  </si>
+  <si>
+    <t>Checklogin</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>password$1</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>DataA2_1</t>
-  </si>
-  <si>
-    <t>DataA2_2</t>
-  </si>
-  <si>
-    <t>DataA2_3</t>
-  </si>
-  <si>
-    <t>Dummy Data_A2_1</t>
-  </si>
-  <si>
-    <t>Dummy Data_A2_2</t>
-  </si>
-  <si>
-    <t>Dummy Data_A2_3</t>
-  </si>
-  <si>
-    <t>Dummy Data_A2_4</t>
-  </si>
-  <si>
-    <t>Dummy Data_A2_5</t>
-  </si>
-  <si>
-    <t>Dummy Data_A2_6</t>
-  </si>
-  <si>
-    <t>Login into application</t>
-  </si>
-  <si>
-    <t>Search for a keyword</t>
-  </si>
-  <si>
-    <t>TestCase_A2</t>
-  </si>
-  <si>
-    <t>Checklogin</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>sam</t>
-  </si>
-  <si>
-    <t>password$1</t>
+    <t>khan</t>
+  </si>
+  <si>
+    <t>NewCustomerRegistration</t>
+  </si>
+  <si>
+    <t>Enter New Customer Registration Details</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>PreferredName</t>
+  </si>
+  <si>
+    <t>DateofBirth</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>PreferredPhone</t>
+  </si>
+  <si>
+    <t>RadioButton</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>Ext</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country </t>
+  </si>
+  <si>
+    <t>PreviousOptician</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,15 +486,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -491,32 +508,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -529,76 +546,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -607,70 +639,82 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
scroll down functionality done
Elements from the mandate page are being read till 24
</commit_message>
<xml_diff>
--- a/src/com/qtpselenium/xls/Login Suite.xlsx
+++ b/src/com/qtpselenium/xls/Login Suite.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="18645" windowHeight="2580"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Checklogin" sheetId="2" r:id="rId2"/>
     <sheet name="NewCustomerRegistration" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="29">
   <si>
     <t>TCID</t>
   </si>
@@ -72,9 +72,6 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>PreferredName</t>
-  </si>
-  <si>
     <t>DateofBirth</t>
   </si>
   <si>
@@ -87,40 +84,32 @@
     <t>PreferredPhone</t>
   </si>
   <si>
-    <t>RadioButton</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>PostCode</t>
-  </si>
-  <si>
-    <t>Ext</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country </t>
-  </si>
-  <si>
-    <t>PreviousOptician</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>m</t>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>Gupte</t>
+  </si>
+  <si>
+    <t>Aakar</t>
+  </si>
+  <si>
+    <t>26/04/1990</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -485,16 +474,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -519,10 +508,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -533,9 +522,11 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -547,15 +538,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -598,10 +589,10 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,10 +617,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -639,28 +630,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -672,48 +659,45 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>1236547890</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>